<commit_message>
Fixed UI, Edit Bug
</commit_message>
<xml_diff>
--- a/dataExcel.xlsx
+++ b/dataExcel.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C30"/>
+  <dimension ref="A1:C27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -788,47 +788,6 @@
         </is>
       </c>
     </row>
-    <row r="28">
-      <c r="A28" t="n">
-        <v>27</v>
-      </c>
-      <c r="B28" t="n">
-        <v>123</v>
-      </c>
-      <c r="C28" t="inlineStr">
-        <is>
-          <t>123</t>
-        </is>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" t="n">
-        <v>28</v>
-      </c>
-      <c r="B29" t="n">
-        <v>1234</v>
-      </c>
-      <c r="C29" t="inlineStr">
-        <is>
-          <t>1234</t>
-        </is>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" t="n">
-        <v>29</v>
-      </c>
-      <c r="B30" t="inlineStr">
-        <is>
-          <t>12345</t>
-        </is>
-      </c>
-      <c r="C30" t="inlineStr">
-        <is>
-          <t>12345</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Fixing target insert update value
</commit_message>
<xml_diff>
--- a/dataExcel.xlsx
+++ b/dataExcel.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C27"/>
+  <dimension ref="A1:C29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -455,7 +455,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>71190504</v>
+        <v>1</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
@@ -468,11 +468,11 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>71190510</v>
+        <v>2</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Joshua Benevan Wisnuwardhana</t>
+          <t>1</t>
         </is>
       </c>
     </row>
@@ -481,11 +481,11 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>71231014</v>
+        <v>3</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Fransina Riyanty Batlayar</t>
+          <t>3</t>
         </is>
       </c>
     </row>
@@ -785,6 +785,30 @@
       <c r="C27" t="inlineStr">
         <is>
           <t>Richard Vanuella</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr"/>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>NIM</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>Nama</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr"/>
+      <c r="B29" t="n">
+        <v>6</v>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>6</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
auto correction and sort table
</commit_message>
<xml_diff>
--- a/dataExcel.xlsx
+++ b/dataExcel.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C30"/>
+  <dimension ref="A1:B27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,15 +436,10 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>NIM</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>NIM</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>Nama</t>
         </is>
@@ -452,374 +447,261 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>1</v>
-      </c>
-      <c r="B2" t="n">
-        <v>1</v>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Stefanus Aditya Dwi Cahyono</t>
+        <v>71190510</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Joshua Benevan Wisnuwardhana</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>2</v>
-      </c>
-      <c r="B3" t="n">
-        <v>2</v>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>1</t>
+        <v>71231014</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Fransina Riyanty Batlayar</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>3</v>
-      </c>
-      <c r="B4" t="n">
-        <v>3</v>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>3</t>
+        <v>71231038</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Amelia Agustin</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>4</v>
-      </c>
-      <c r="B5" t="n">
-        <v>71231038</v>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>Amelia Agustin</t>
+        <v>71241071</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Jeremy Fidelo</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>5</v>
-      </c>
-      <c r="B6" t="n">
-        <v>71241071</v>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>Jeremy Fidelo</t>
+        <v>71241072</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Gilbert Danelle Lo</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>6</v>
-      </c>
-      <c r="B7" t="n">
-        <v>71241072</v>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>Gilbert Danelle Lo</t>
+        <v>71241073</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Stefanus Westin Giovanno Mursito</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>7</v>
-      </c>
-      <c r="B8" t="n">
-        <v>71241073</v>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>Stefanus Westin Giovanno Mursito</t>
+        <v>71241075</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Giovanni Albert Harjanto</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>8</v>
-      </c>
-      <c r="B9" t="n">
-        <v>71241075</v>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>Giovanni Albert Harjanto</t>
+        <v>71241078</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Kevin Setiadi Wijaya</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>9</v>
-      </c>
-      <c r="B10" t="n">
-        <v>71241078</v>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>Kevin Setiadi Wijaya</t>
+        <v>71241079</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Natalie Neysa Jessica Soesanto</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>10</v>
-      </c>
-      <c r="B11" t="n">
-        <v>71241079</v>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>Natalie Neysa Jessica Soesanto</t>
+        <v>71241083</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Ignacia Aurelia Robetta</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>11</v>
-      </c>
-      <c r="B12" t="n">
-        <v>71241083</v>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>Ignacia Aurelia Robetta</t>
+        <v>71241085</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Samuel Kristos Xavier</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>12</v>
-      </c>
-      <c r="B13" t="n">
-        <v>71241085</v>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>Samuel Kristos Xavier</t>
+        <v>71241091</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Abel Lalang Buana</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>13</v>
-      </c>
-      <c r="B14" t="n">
-        <v>71241091</v>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>Abel Lalang Buana</t>
+        <v>71241099</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Listyan Aji Maharsi Pratama</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>14</v>
-      </c>
-      <c r="B15" t="n">
-        <v>71241099</v>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>Listyan Aji Maharsi Pratama</t>
+        <v>71241105</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Audris Kasula</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>15</v>
-      </c>
-      <c r="B16" t="n">
-        <v>71241105</v>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>Audris Kasula</t>
+        <v>71241106</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Hervian Paskah Pradana</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>16</v>
-      </c>
-      <c r="B17" t="n">
-        <v>71241106</v>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>Hervian Paskah Pradana</t>
+        <v>71241114</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Hendrikus Lanang Ona</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>17</v>
-      </c>
-      <c r="B18" t="n">
-        <v>71241114</v>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>Hendrikus Lanang Ona</t>
+        <v>71241115</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Devon Novan Surya Putra</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>18</v>
-      </c>
-      <c r="B19" t="n">
-        <v>71241115</v>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>Devon Novan Surya Putra</t>
+        <v>71241116</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Putra Eka Setiawan</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>19</v>
-      </c>
-      <c r="B20" t="n">
-        <v>71241116</v>
-      </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>Putra Eka Setiawan</t>
+        <v>71241117</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Winlardo Thie</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>20</v>
-      </c>
-      <c r="B21" t="n">
-        <v>71241117</v>
-      </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>Winlardo Thie</t>
+        <v>71241119</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Antonius Kiya Ananda Derron</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>21</v>
-      </c>
-      <c r="B22" t="n">
-        <v>71241119</v>
-      </c>
-      <c r="C22" t="inlineStr">
-        <is>
-          <t>Antonius Kiya Ananda Derron</t>
+        <v>71241123</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Fransiska</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>22</v>
-      </c>
-      <c r="B23" t="n">
-        <v>71241123</v>
-      </c>
-      <c r="C23" t="inlineStr">
-        <is>
-          <t>Fransiska</t>
+        <v>71241151</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Harrison Abraham Pribadi</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>23</v>
-      </c>
-      <c r="B24" t="n">
-        <v>71241151</v>
-      </c>
-      <c r="C24" t="inlineStr">
-        <is>
-          <t>Harrison Abraham Pribadi</t>
+        <v>71241153</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Felix Benedictus Setiawan</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>24</v>
-      </c>
-      <c r="B25" t="n">
-        <v>71241153</v>
-      </c>
-      <c r="C25" t="inlineStr">
-        <is>
-          <t>Felix Benedictus Setiawan</t>
+        <v>71241156</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Jochelino Felix Kurniawan</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>25</v>
-      </c>
-      <c r="B26" t="n">
-        <v>71241156</v>
-      </c>
-      <c r="C26" t="inlineStr">
-        <is>
-          <t>Jochelino Felix Kurniawan</t>
+        <v>71241159</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>Richard Vanuella</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>26</v>
-      </c>
-      <c r="B27" t="n">
-        <v>71241159</v>
-      </c>
-      <c r="C27" t="inlineStr">
-        <is>
-          <t>Richard Vanuella</t>
-        </is>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="inlineStr"/>
-      <c r="B28" t="inlineStr">
-        <is>
-          <t>NIM</t>
-        </is>
-      </c>
-      <c r="C28" t="inlineStr">
-        <is>
-          <t>Nama</t>
-        </is>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" t="inlineStr"/>
-      <c r="B29" t="n">
-        <v>6</v>
-      </c>
-      <c r="C29" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" t="inlineStr"/>
-      <c r="B30" t="n">
-        <v>7</v>
-      </c>
-      <c r="C30" t="inlineStr">
-        <is>
-          <t>7</t>
+        <v>71190504</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Stefanus Aditya Dwi Cahyono</t>
         </is>
       </c>
     </row>

</xml_diff>